<commit_message>
Download files from url
</commit_message>
<xml_diff>
--- a/candidatos.xlsx
+++ b/candidatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2019201410840742\Documents\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2019201410840742\Documents\file-magic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Alessandra Vieira Nunes</t>
   </si>
@@ -36,38 +36,38 @@
     <t>Jucira Alves Nogueira</t>
   </si>
   <si>
-    <t>Alexandre Soares Silva</t>
-  </si>
-  <si>
-    <t>Camila Oliveira dos Santos</t>
-  </si>
-  <si>
-    <t>Bárbara Carvalho Monteiro</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample3.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample4.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample5.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample6.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\2019201410840742\Documents\project\pdfs\sample2.pdf</t>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Inscrição</t>
+  </si>
+  <si>
+    <t>http://www.africau.edu/images/default/sample.pdf</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/ER/tests/xhtml/testfiles/resources/pdf/dummy.pdf</t>
+  </si>
+  <si>
+    <t>https://juventudedesporto.cplp.org/files/sample-pdf_9359.pdf</t>
+  </si>
+  <si>
+    <t>Ana Clara</t>
+  </si>
+  <si>
+    <t>545454</t>
+  </si>
+  <si>
+    <t>https://via.placeholder.com/300.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -80,6 +80,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +112,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -121,6 +129,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -414,88 +425,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5">
-        <v>1255463</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3">
-        <v>21458799662</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>1255487</v>
+        <v>1255463</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>21458799662</v>
       </c>
       <c r="C3" s="5">
-        <v>1255498</v>
+        <v>1255487</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>1255520</v>
+        <v>1255498</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5">
-        <v>1255521</v>
+        <v>202069</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1255600</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>